<commit_message>
Alignment & other styling. Also defining a validation function.
With this update, the entry field now only accepts numeric input, thanks to the validation function. This should help in maintaining data integrity and prevent users from accidentally entering non-numeric values.
</commit_message>
<xml_diff>
--- a/Build Room/EUC_Build_Room.xlsx
+++ b/Build Room/EUC_Build_Room.xlsx
@@ -311,8 +311,11 @@
           <t>Desktop Mini</t>
         </is>
       </c>
+      <c r="B2" s="3" t="n">
+        <v>147</v>
+      </c>
       <c r="C2" s="3" t="n">
-        <v>138</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" ht="24" customHeight="1" s="4">
@@ -322,10 +325,10 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>25</v>
+        <v>-1</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>20</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" ht="24" customHeight="1" s="4">
@@ -335,10 +338,10 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" ht="24" customHeight="1" s="4">
@@ -347,9 +350,11 @@
           <t>Laptop 840 G9</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n"/>
+      <c r="B5" s="3" t="n">
+        <v>12</v>
+      </c>
       <c r="C5" s="3" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" ht="24" customHeight="1" s="4">
@@ -375,7 +380,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" ht="24" customHeight="1" s="4">
@@ -384,8 +389,11 @@
           <t xml:space="preserve">Monitor 24” </t>
         </is>
       </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="C8" s="3" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="24" customHeight="1" s="4">
@@ -407,8 +415,11 @@
           <t>USB External DVD-RW Drive</t>
         </is>
       </c>
+      <c r="B10" s="3" t="n">
+        <v>46</v>
+      </c>
       <c r="C10" s="3" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" ht="35.25" customHeight="1" s="4">
@@ -417,8 +428,11 @@
           <t>Wired Headset Poly 3325</t>
         </is>
       </c>
+      <c r="B11" s="3" t="n">
+        <v>30</v>
+      </c>
       <c r="C11" s="3" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="35.25" customHeight="1" s="4">
@@ -440,8 +454,11 @@
           <t xml:space="preserve">Wireless Headset Poly </t>
         </is>
       </c>
+      <c r="B13" s="3" t="n">
+        <v>6</v>
+      </c>
       <c r="C13" s="3" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" ht="24" customHeight="1" s="4">
@@ -450,8 +467,11 @@
           <t>Wireless Keyboard and Mouse</t>
         </is>
       </c>
+      <c r="B14" s="3" t="n">
+        <v>5</v>
+      </c>
       <c r="C14" s="3" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -475,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
@@ -637,19 +657,325 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>2023-12-05 08:04:53</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>Desktop Mini</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:12:00</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:13:29</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Laptop x360 G8</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:13:52</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Add 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:58:55</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:03</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:09</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monitor 24” </t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:12</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Wired Headset Poly 3325</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:15</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>USB External DVD-RW Drive</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:19</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Wireless Keyboard and Mouse</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-05 21:59:22</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wireless Headset Poly </t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Add 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:09:25</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:09:39</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:09:53</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:09:59</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:10:03</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G10</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Subtract 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:20:13</t>
+        </is>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Desktop Mini</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Add 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:20:17</t>
+        </is>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>Laptop 840 G9</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Add 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-12-07 22:44:46</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Dock Thunderbolt G4</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Add 400</t>
         </is>
       </c>
     </row>

</xml_diff>